<commit_message>
Misschien werkende versie van het programma, testen op een goede origin moet nog gebeuren.
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -1,42 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91695C7D-3734-44C9-9882-FA36D341EA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F862F173-A21F-47FC-8AE4-F2E4F65A076B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3495" windowWidth="28800" windowHeight="11070" xr2:uid="{B6893147-27E0-43F2-AE90-F162BB8ACF10}"/>
+    <workbookView xWindow="4680" yWindow="1110" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>Id</t>
   </si>
@@ -116,6 +100,9 @@
     <t>Kevin Van Weyenberg</t>
   </si>
   <si>
+    <t>Sint-Denijs-Westrem</t>
+  </si>
+  <si>
     <t>OK</t>
   </si>
   <si>
@@ -125,26 +112,35 @@
     <t>Wachtebeke</t>
   </si>
   <si>
-    <t>AS-Out Kit EOS 2nd GEN</t>
-  </si>
-  <si>
-    <t>Sint-Denijs-Westrem</t>
-  </si>
-  <si>
-    <t>342CC4E28CEC</t>
+    <t>DAAZ03330111</t>
+  </si>
+  <si>
+    <t>1908220400048819</t>
+  </si>
+  <si>
+    <t>1908320020042470</t>
+  </si>
+  <si>
+    <t>1908222340013186</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,7 +151,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -167,16 +170,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -189,7 +208,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -223,20 +242,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -264,31 +283,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -316,23 +318,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -344,157 +329,182 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63E35CC-B829-4C61-A187-625C9D901B19}">
-  <dimension ref="A1:V3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
@@ -503,21 +513,23 @@
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -544,7 +556,7 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
@@ -553,13 +565,13 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
@@ -577,15 +589,15 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>845212</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>45260</v>
       </c>
       <c r="C2" t="s">
@@ -601,44 +613,44 @@
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1">
         <v>9185</v>
       </c>
       <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>9185</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2">
-        <v>539094977</v>
+        <v>29</v>
+      </c>
+      <c r="P2" s="1">
+        <v>934517804</v>
       </c>
       <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="2">
-        <v>767181911022</v>
+      <c r="V2" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>845212</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>45260</v>
       </c>
       <c r="C3" t="s">
@@ -648,43 +660,150 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1">
         <v>9185</v>
       </c>
       <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>9185</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3">
-        <v>539094977</v>
+        <v>29</v>
+      </c>
+      <c r="P3" s="1">
+        <v>934517804</v>
       </c>
       <c r="Q3" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3" s="6" t="s">
         <v>31</v>
+      </c>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="1">
+        <v>934517804</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="1">
+        <v>934517804</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit einde van de dag 18/01
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F862F173-A21F-47FC-8AE4-F2E4F65A076B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C116FE-B955-4948-BB8F-8AA2127F643C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1110" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="1455" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Id</t>
   </si>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t>Wachtebeke</t>
-  </si>
-  <si>
-    <t>DAAZ03330111</t>
-  </si>
-  <si>
-    <t>1908220400048819</t>
   </si>
   <si>
     <t>1908320020042470</t>
@@ -495,10 +489,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +519,7 @@
     <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +587,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>845212</v>
       </c>
@@ -643,10 +637,10 @@
         <v>25</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>845212</v>
       </c>
@@ -697,113 +691,6 @@
       </c>
       <c r="V3" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>845212</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45260</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="1">
-        <v>9185</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="1">
-        <v>9185</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="1">
-        <v>934517804</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>845212</v>
-      </c>
-      <c r="B5" s="2">
-        <v>45260</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="1">
-        <v>9185</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="1">
-        <v>9185</v>
-      </c>
-      <c r="O5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="1">
-        <v>934517804</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In orde zetten van de applicatie voor het gebruik met de ingebouwde GUI
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C116FE-B955-4948-BB8F-8AA2127F643C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4001475-3CC1-418C-80EA-85198DC295FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="1455" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Id</t>
   </si>
@@ -91,9 +91,6 @@
     <t>02. Telenet Center</t>
   </si>
   <si>
-    <t>David Vander Auwera</t>
-  </si>
-  <si>
     <t>Origin Center only</t>
   </si>
   <si>
@@ -112,17 +109,20 @@
     <t>Wachtebeke</t>
   </si>
   <si>
-    <t>1908320020042470</t>
-  </si>
-  <si>
-    <t>1908222340013186</t>
+    <t>Klant 1</t>
+  </si>
+  <si>
+    <t>Klant 3</t>
+  </si>
+  <si>
+    <t>38437D095779</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +135,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -181,7 +188,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -491,13 +499,13 @@
   </sheetPr>
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -598,46 +606,46 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
       </c>
       <c r="K2" s="1">
         <v>9185</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="1">
         <v>9185</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="1">
-        <v>934517804</v>
+        <v>28</v>
+      </c>
+      <c r="P2" s="6">
+        <v>509514324</v>
       </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -651,46 +659,46 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
       </c>
       <c r="K3" s="1">
         <v>9185</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N3" s="1">
         <v>9185</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="1">
-        <v>934517804</v>
+        <v>28</v>
+      </c>
+      <c r="P3" s="6">
+        <v>504798205</v>
       </c>
       <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="V3" s="7">
+        <v>958330964654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eerste versie van de applicatie als executabel
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4001475-3CC1-418C-80EA-85198DC295FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855F06EF-1AB0-4420-A4A9-BAD12143817D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="4530" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tweede versie van de applicatie als executable
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E915E9-EE00-4AB9-B600-C0DEC2AD8552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47A61D5-84A0-46B8-BCA3-37DBD602ABDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="10455" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8175" yWindow="4530" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
     <t>Klant 3</t>
   </si>
   <si>
-    <t>38437D095779</t>
+    <t>38437D095778</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
         <v>28</v>
       </c>
       <c r="P2" s="6">
-        <v>509514334</v>
+        <v>509514324</v>
       </c>
       <c r="Q2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Progress van dag 25/01/2024
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47A61D5-84A0-46B8-BCA3-37DBD602ABDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB9075-1246-4A5E-AF7D-F6DA0019A05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8175" yWindow="4530" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -115,14 +115,176 @@
     <t>Klant 3</t>
   </si>
   <si>
-    <t>38437D095778</t>
+    <t>6802B83086EA</t>
+  </si>
+  <si>
+    <t>6802B8302B43</t>
+  </si>
+  <si>
+    <t>DAAZ81060223</t>
+  </si>
+  <si>
+    <t>DC537CFA32EF</t>
+  </si>
+  <si>
+    <t>5C353B9D6AE9</t>
+  </si>
+  <si>
+    <t>1907218510096975</t>
+  </si>
+  <si>
+    <t>905C44BBAE58</t>
+  </si>
+  <si>
+    <t>1908220370014258</t>
+  </si>
+  <si>
+    <t>6802B8F67454</t>
+  </si>
+  <si>
+    <t>DAAZ802409A0</t>
+  </si>
+  <si>
+    <t>1907318230064633</t>
+  </si>
+  <si>
+    <t>XBAN30580875</t>
+  </si>
+  <si>
+    <t>226150556874 </t>
+  </si>
+  <si>
+    <t>38437D079B18</t>
+  </si>
+  <si>
+    <t>94988FF4B35B</t>
+  </si>
+  <si>
+    <t>Klant 2</t>
+  </si>
+  <si>
+    <t>Klant 4</t>
+  </si>
+  <si>
+    <t>Klant 5</t>
+  </si>
+  <si>
+    <t>Klant 6</t>
+  </si>
+  <si>
+    <t>Klant 7</t>
+  </si>
+  <si>
+    <t>Klant 8</t>
+  </si>
+  <si>
+    <t>Klant 9</t>
+  </si>
+  <si>
+    <t>Klant 10</t>
+  </si>
+  <si>
+    <t>Klant 11</t>
+  </si>
+  <si>
+    <t>Klant 12</t>
+  </si>
+  <si>
+    <t>Klant 13</t>
+  </si>
+  <si>
+    <t>Klant 14</t>
+  </si>
+  <si>
+    <t>Klant 15</t>
+  </si>
+  <si>
+    <t>Klant 16</t>
+  </si>
+  <si>
+    <t>Klant 17</t>
+  </si>
+  <si>
+    <t>Klant 18</t>
+  </si>
+  <si>
+    <t>Klant 19</t>
+  </si>
+  <si>
+    <t>Klant 20</t>
+  </si>
+  <si>
+    <t>Klant 21</t>
+  </si>
+  <si>
+    <t>Klant 22</t>
+  </si>
+  <si>
+    <t>Klant 23</t>
+  </si>
+  <si>
+    <t>Klant 24</t>
+  </si>
+  <si>
+    <t>Klant 25</t>
+  </si>
+  <si>
+    <t>Oostakker</t>
+  </si>
+  <si>
+    <t>Sint-Niklaas</t>
+  </si>
+  <si>
+    <t>Aartselaar</t>
+  </si>
+  <si>
+    <t>Lokeren</t>
+  </si>
+  <si>
+    <t>Eeklo</t>
+  </si>
+  <si>
+    <t>6802B85924BE</t>
+  </si>
+  <si>
+    <t>1908320370045662</t>
+  </si>
+  <si>
+    <t>1908220370045665</t>
+  </si>
+  <si>
+    <t>B4F2671C8F16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1908322140006972 </t>
+  </si>
+  <si>
+    <t>1908322140006989</t>
+  </si>
+  <si>
+    <t>Klant 26</t>
+  </si>
+  <si>
+    <t>Klant 27</t>
+  </si>
+  <si>
+    <t>Klant 28</t>
+  </si>
+  <si>
+    <t>Klant 29</t>
+  </si>
+  <si>
+    <t>Klant 30</t>
+  </si>
+  <si>
+    <t>Klant 31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,7 +300,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,18 +336,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -188,13 +360,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="8">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{9750B42F-0F1B-43D0-B441-6C53333F40A3}"/>
+    <cellStyle name="Standaard 3" xfId="2" xr:uid="{A4069E7E-EE2A-4DC7-ADF8-25EA4E04F358}"/>
+    <cellStyle name="Standaard 4" xfId="3" xr:uid="{2AAA64FB-B566-4C79-B72D-5BFFAD343B9F}"/>
+    <cellStyle name="Standaard 5" xfId="4" xr:uid="{1C465A9E-EC45-4D23-A852-72347BE4DFC1}"/>
+    <cellStyle name="Standaard 6" xfId="5" xr:uid="{82F7BAEE-9F72-49D2-A25E-6848EAD997EF}"/>
+    <cellStyle name="Standaard 7" xfId="6" xr:uid="{654A8370-722E-4488-9399-EAD2A9976AC0}"/>
+    <cellStyle name="Standaard 8" xfId="7" xr:uid="{6E6C2A24-65CA-45BD-BC51-541A2285BD03}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,16 +678,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
@@ -515,15 +696,15 @@
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -591,11 +772,11 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>845212</v>
       </c>
@@ -615,7 +796,7 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
         <v>26</v>
@@ -639,7 +820,7 @@
         <v>28</v>
       </c>
       <c r="P2" s="6">
-        <v>509514324</v>
+        <v>556918931</v>
       </c>
       <c r="Q2" t="s">
         <v>24</v>
@@ -648,7 +829,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>845212</v>
       </c>
@@ -659,49 +840,1587 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="6">
+        <v>525743535</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="6">
+        <v>525743535</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1">
-        <v>9185</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="1">
-        <v>9185</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="6">
-        <v>504798215</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="7">
-        <v>958330964654</v>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="6">
+        <v>1140921272</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+      <c r="V5" s="6">
+        <v>226202634157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1140921272</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="6">
+        <v>14348320</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+      <c r="V7" s="6">
+        <v>973278351717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="6">
+        <v>518994052</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="6">
+        <v>518994052</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="6">
+        <v>1097032210</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+      <c r="V10" s="6">
+        <v>226151377291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="6">
+        <v>1097032210</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="6">
+        <v>1097032210</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="6">
+        <v>908533928</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>24</v>
+      </c>
+      <c r="V13" s="6">
+        <v>226255643236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O14" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="6">
+        <v>33363552</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>24</v>
+      </c>
+      <c r="V14" s="6">
+        <v>226343983036</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="6">
+        <v>33363552</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O16" t="s">
+        <v>28</v>
+      </c>
+      <c r="P16" s="6">
+        <v>33363552</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>24</v>
+      </c>
+      <c r="V16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O17" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="6">
+        <v>913393325</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O18" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18" s="6">
+        <v>635262393</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>24</v>
+      </c>
+      <c r="V18" s="6">
+        <v>982018817676</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L19" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O19" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="6">
+        <v>1208511840</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>24</v>
+      </c>
+      <c r="V19" s="6">
+        <v>226400339703</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" s="6">
+        <v>973316386</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>24</v>
+      </c>
+      <c r="V20" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L21" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O21" t="s">
+        <v>28</v>
+      </c>
+      <c r="P21" s="6">
+        <v>33456613</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O22" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="6">
+        <v>33456613</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>24</v>
+      </c>
+      <c r="V22" s="6">
+        <v>226162027679</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O23" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="6">
+        <v>820808037</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>24</v>
+      </c>
+      <c r="V23" s="6">
+        <v>964214570814</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L24" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O24" t="s">
+        <v>28</v>
+      </c>
+      <c r="P24" s="6">
+        <v>822119153</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L25" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" t="s">
+        <v>27</v>
+      </c>
+      <c r="N25" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O25" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="6">
+        <v>822119153</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>24</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O26" t="s">
+        <v>28</v>
+      </c>
+      <c r="P26" s="6">
+        <v>1208816335</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>24</v>
+      </c>
+      <c r="V26" s="6">
+        <v>226420241029</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L27" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" s="6">
+        <v>1120339690</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>24</v>
+      </c>
+      <c r="V27" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M28" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P28" s="6">
+        <v>1120339690</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>24</v>
+      </c>
+      <c r="V28" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L29" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O29" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" s="6">
+        <v>1120339690</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>24</v>
+      </c>
+      <c r="V29" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L30" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O30" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" s="6">
+        <v>1207587935</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>24</v>
+      </c>
+      <c r="V30" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B31" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L31" t="s">
+        <v>28</v>
+      </c>
+      <c r="M31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O31" t="s">
+        <v>28</v>
+      </c>
+      <c r="P31" s="6">
+        <v>509514324</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>24</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>845212</v>
+      </c>
+      <c r="B32" s="2">
+        <v>45260</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32" s="1">
+        <v>9185</v>
+      </c>
+      <c r="L32" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32" s="1">
+        <v>9185</v>
+      </c>
+      <c r="O32" t="s">
+        <v>28</v>
+      </c>
+      <c r="P32" s="6">
+        <v>509514324</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>24</v>
+      </c>
+      <c r="V32" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning up print statements, only 1 left behind to see what serial numbers are found in the table before editing the interaction
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D473333-5D01-49D9-96FB-621748B2BE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1133AF-C6CF-4831-8BDB-C50F6B9818E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4545" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="3450" windowWidth="16515" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -118,18 +118,6 @@
     <t>Dorp  27 107</t>
   </si>
   <si>
-    <t>B4F267004A9A</t>
-  </si>
-  <si>
-    <t>DAAZ821102A6</t>
-  </si>
-  <si>
-    <t>20B82B2124DA</t>
-  </si>
-  <si>
-    <t>DC537C9D492A</t>
-  </si>
-  <si>
     <t>Dorp  27 108</t>
   </si>
   <si>
@@ -151,13 +139,19 @@
     <t>Dorp  27 111</t>
   </si>
   <si>
-    <t>Klant 7</t>
-  </si>
-  <si>
-    <t>Dorp  27 112</t>
-  </si>
-  <si>
     <t>Sint-Denijs-Westrem</t>
+  </si>
+  <si>
+    <t>DC537CF69DF4</t>
+  </si>
+  <si>
+    <t>AC220594A0BB</t>
+  </si>
+  <si>
+    <t>1907318070029335</t>
+  </si>
+  <si>
+    <t>1907218070029338</t>
   </si>
 </sst>
 </file>
@@ -216,8 +210,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -250,10 +246,12 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 10" xfId="9" xr:uid="{970D2C42-7879-4698-9EDC-BE237EBCC052}"/>
     <cellStyle name="Standaard 11" xfId="10" xr:uid="{EEADE249-AA4C-4C58-86DA-A5AD80643891}"/>
+    <cellStyle name="Standaard 12" xfId="11" xr:uid="{E6C75EA0-9867-4EE0-B4B0-A782B2BF660C}"/>
+    <cellStyle name="Standaard 13" xfId="12" xr:uid="{BEF4C3B7-2CD0-4374-B56B-BB3D68024C77}"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{9750B42F-0F1B-43D0-B441-6C53333F40A3}"/>
     <cellStyle name="Standaard 3" xfId="2" xr:uid="{A4069E7E-EE2A-4DC7-ADF8-25EA4E04F358}"/>
     <cellStyle name="Standaard 4" xfId="3" xr:uid="{2AAA64FB-B566-4C79-B72D-5BFFAD343B9F}"/>
@@ -564,10 +562,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +680,7 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
@@ -706,13 +704,13 @@
         <v>27</v>
       </c>
       <c r="P2" s="6">
-        <v>611983407</v>
+        <v>1011782546</v>
       </c>
       <c r="Q2" t="s">
         <v>24</v>
       </c>
       <c r="V2" s="6">
-        <v>958255663658</v>
+        <v>226415171533</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -735,7 +733,7 @@
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
         <v>25</v>
@@ -759,13 +757,13 @@
         <v>27</v>
       </c>
       <c r="P3" s="6">
-        <v>1112532911</v>
+        <v>1011782546</v>
       </c>
       <c r="Q3" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="6">
-        <v>226254516167</v>
+      <c r="V3" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -788,13 +786,13 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K4" s="1">
         <v>9187</v>
@@ -803,7 +801,7 @@
         <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N4" s="1">
         <v>9187</v>
@@ -812,13 +810,13 @@
         <v>27</v>
       </c>
       <c r="P4" s="6">
-        <v>1160669058</v>
+        <v>693300224</v>
       </c>
       <c r="Q4" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="6" t="s">
-        <v>32</v>
+      <c r="V4" s="6">
+        <v>965346592830</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -832,7 +830,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -841,13 +839,13 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K5" s="1">
         <v>9188</v>
@@ -856,7 +854,7 @@
         <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N5" s="1">
         <v>9188</v>
@@ -865,13 +863,13 @@
         <v>27</v>
       </c>
       <c r="P5" s="6">
-        <v>1160669058</v>
+        <v>693300224</v>
       </c>
       <c r="Q5" t="s">
         <v>24</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -885,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -894,13 +892,13 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1">
         <v>9189</v>
@@ -909,7 +907,7 @@
         <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N6" s="1">
         <v>9189</v>
@@ -918,13 +916,13 @@
         <v>27</v>
       </c>
       <c r="P6" s="6">
-        <v>1208924358</v>
+        <v>693300224</v>
       </c>
       <c r="Q6" t="s">
         <v>24</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -938,7 +936,7 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
@@ -947,13 +945,13 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K7" s="1">
         <v>9190</v>
@@ -962,7 +960,7 @@
         <v>27</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N7" s="1">
         <v>9190</v>
@@ -971,66 +969,13 @@
         <v>27</v>
       </c>
       <c r="P7" s="6">
-        <v>935253485</v>
+        <v>693300224</v>
       </c>
       <c r="Q7" t="s">
         <v>24</v>
       </c>
-      <c r="V7" s="6">
-        <v>963430829813</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>845218</v>
-      </c>
-      <c r="B8" s="2">
-        <v>45266</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="V7" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="1">
-        <v>9191</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="1">
-        <v>9191</v>
-      </c>
-      <c r="O8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="6">
-        <v>1003938983</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>24</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully working first version of the application
</commit_message>
<xml_diff>
--- a/excel/TestReturnRental_Case1.xlsx
+++ b/excel/TestReturnRental_Case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kassa\Documents\Scripts\ReturnRental\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1133AF-C6CF-4831-8BDB-C50F6B9818E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EA3DD0-ED3C-461D-9E8B-C846C9581430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="3450" windowWidth="16515" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="900" windowWidth="16515" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Id</t>
   </si>
@@ -127,31 +127,16 @@
     <t>Dorp  27 109</t>
   </si>
   <si>
+    <t>Sint-Denijs-Westrem</t>
+  </si>
+  <si>
+    <t>6802B874E598</t>
+  </si>
+  <si>
     <t>Klant 5</t>
   </si>
   <si>
     <t>Dorp  27 110</t>
-  </si>
-  <si>
-    <t>Klant 6</t>
-  </si>
-  <si>
-    <t>Dorp  27 111</t>
-  </si>
-  <si>
-    <t>Sint-Denijs-Westrem</t>
-  </si>
-  <si>
-    <t>DC537CF69DF4</t>
-  </si>
-  <si>
-    <t>AC220594A0BB</t>
-  </si>
-  <si>
-    <t>1907318070029335</t>
-  </si>
-  <si>
-    <t>1907218070029338</t>
   </si>
 </sst>
 </file>
@@ -210,8 +195,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
@@ -246,12 +237,18 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 10" xfId="9" xr:uid="{970D2C42-7879-4698-9EDC-BE237EBCC052}"/>
     <cellStyle name="Standaard 11" xfId="10" xr:uid="{EEADE249-AA4C-4C58-86DA-A5AD80643891}"/>
     <cellStyle name="Standaard 12" xfId="11" xr:uid="{E6C75EA0-9867-4EE0-B4B0-A782B2BF660C}"/>
     <cellStyle name="Standaard 13" xfId="12" xr:uid="{BEF4C3B7-2CD0-4374-B56B-BB3D68024C77}"/>
+    <cellStyle name="Standaard 14" xfId="13" xr:uid="{6FFDBEEE-F6E2-4F84-A631-06A2478AD086}"/>
+    <cellStyle name="Standaard 15" xfId="14" xr:uid="{8C3BF45F-E7BA-4926-80D5-CDA047C0D8D6}"/>
+    <cellStyle name="Standaard 16" xfId="15" xr:uid="{63D338E7-79CD-4C69-A440-980C772395AE}"/>
+    <cellStyle name="Standaard 17" xfId="16" xr:uid="{253F92AD-F4D5-4C2C-ADE4-46EB0C1B550C}"/>
+    <cellStyle name="Standaard 18" xfId="17" xr:uid="{D17417BD-85A4-4AF7-A472-C45DB3CBF9E2}"/>
+    <cellStyle name="Standaard 19" xfId="18" xr:uid="{65E92A0A-780C-41AD-908A-4847DB1795A8}"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{9750B42F-0F1B-43D0-B441-6C53333F40A3}"/>
     <cellStyle name="Standaard 3" xfId="2" xr:uid="{A4069E7E-EE2A-4DC7-ADF8-25EA4E04F358}"/>
     <cellStyle name="Standaard 4" xfId="3" xr:uid="{2AAA64FB-B566-4C79-B72D-5BFFAD343B9F}"/>
@@ -565,7 +562,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
@@ -704,13 +701,13 @@
         <v>27</v>
       </c>
       <c r="P2" s="6">
-        <v>1011782546</v>
+        <v>266134856</v>
       </c>
       <c r="Q2" t="s">
         <v>24</v>
       </c>
       <c r="V2" s="6">
-        <v>226415171533</v>
+        <v>973244716178</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -733,7 +730,7 @@
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
         <v>25</v>
@@ -757,13 +754,13 @@
         <v>27</v>
       </c>
       <c r="P3" s="6">
-        <v>1011782546</v>
+        <v>721090219</v>
       </c>
       <c r="Q3" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>40</v>
+      <c r="V3" s="6">
+        <v>973222132639</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -786,7 +783,7 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -810,13 +807,13 @@
         <v>27</v>
       </c>
       <c r="P4" s="6">
-        <v>693300224</v>
+        <v>640547479</v>
       </c>
       <c r="Q4" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="6">
-        <v>965346592830</v>
+      <c r="V4" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -839,7 +836,7 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -863,13 +860,17 @@
         <v>27</v>
       </c>
       <c r="P5" s="6">
-        <v>693300224</v>
+        <v>824035814</v>
       </c>
       <c r="Q5" t="s">
         <v>24</v>
       </c>
-      <c r="V5" s="6" t="s">
-        <v>41</v>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
+        <v>973037989617</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -883,7 +884,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -892,13 +893,13 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K6" s="1">
         <v>9189</v>
@@ -907,7 +908,7 @@
         <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N6" s="1">
         <v>9189</v>
@@ -916,67 +917,25 @@
         <v>27</v>
       </c>
       <c r="P6" s="6">
-        <v>693300224</v>
+        <v>824035814</v>
       </c>
       <c r="Q6" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="6" t="s">
-        <v>42</v>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6">
+        <v>973161507193</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>845217</v>
-      </c>
-      <c r="B7" s="2">
-        <v>45265</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="1">
-        <v>9190</v>
-      </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="1">
-        <v>9190</v>
-      </c>
-      <c r="O7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="6">
-        <v>693300224</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>24</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="K7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="P7" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>